<commit_message>
Cambio en direcciones agrupadas por componente
</commit_message>
<xml_diff>
--- a/03_ips_clean/04_ips_stats.xlsx
+++ b/03_ips_clean/04_ips_stats.xlsx
@@ -1758,49 +1758,49 @@
         <v>198</v>
       </c>
       <c r="D22" t="n">
-        <v>-9.12520303030303</v>
+        <v>90.874795959596</v>
       </c>
       <c r="E22" t="n">
-        <v>4.37635068012405</v>
+        <v>4.37635199353916</v>
       </c>
       <c r="F22" t="n">
-        <v>-9.35635</v>
+        <v>90.64365</v>
       </c>
       <c r="G22" t="n">
-        <v>-8.9257725</v>
+        <v>91.0742275</v>
       </c>
       <c r="H22" t="n">
         <v>4.03007745</v>
       </c>
       <c r="I22" t="n">
-        <v>-21.4792</v>
+        <v>78.5208</v>
       </c>
       <c r="J22" t="n">
-        <v>-1.4</v>
+        <v>98.6</v>
       </c>
       <c r="K22" t="n">
         <v>20.0792</v>
       </c>
       <c r="L22" t="n">
-        <v>-0.365022779954126</v>
+        <v>-0.365022989356409</v>
       </c>
       <c r="M22" t="n">
-        <v>0.100209988636462</v>
+        <v>0.100208204576704</v>
       </c>
       <c r="N22" t="n">
-        <v>0.311013700008604</v>
+        <v>0.311013793348951</v>
       </c>
       <c r="O22" t="n">
-        <v>-11.774525</v>
+        <v>88.225475</v>
       </c>
       <c r="P22" t="n">
-        <v>-9.35635</v>
+        <v>90.64365</v>
       </c>
       <c r="Q22" t="n">
-        <v>-5.79185</v>
+        <v>94.20815</v>
       </c>
       <c r="R22" t="n">
-        <v>-1.4</v>
+        <v>98.6</v>
       </c>
     </row>
     <row r="23">
@@ -1926,49 +1926,49 @@
         <v>198</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.0222853535353535</v>
+        <v>-2.22863131313131</v>
       </c>
       <c r="E25" t="n">
-        <v>0.0145799472061553</v>
+        <v>1.45828729917437</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.01985</v>
+        <v>-1.9813</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.0206175</v>
+        <v>-2.061786875</v>
       </c>
       <c r="H25" t="n">
-        <v>0.01178667</v>
+        <v>1.16880771</v>
       </c>
       <c r="I25" t="n">
-        <v>-0.0798</v>
+        <v>-7.983</v>
       </c>
       <c r="J25" t="n">
-        <v>0</v>
+        <v>-0.0032</v>
       </c>
       <c r="K25" t="n">
-        <v>0.0798</v>
+        <v>7.9798</v>
       </c>
       <c r="L25" t="n">
-        <v>-1.32711682260432</v>
+        <v>-1.32785639044366</v>
       </c>
       <c r="M25" t="n">
-        <v>2.42986023466552</v>
+        <v>2.43244052505035</v>
       </c>
       <c r="N25" t="n">
-        <v>0.0010361517295931</v>
+        <v>0.103635965612088</v>
       </c>
       <c r="O25" t="n">
-        <v>-0.029</v>
+        <v>-2.900325</v>
       </c>
       <c r="P25" t="n">
-        <v>-0.01985</v>
+        <v>-1.9813</v>
       </c>
       <c r="Q25" t="n">
-        <v>-0.0124</v>
+        <v>-1.23915</v>
       </c>
       <c r="R25" t="n">
-        <v>0</v>
+        <v>-0.0032</v>
       </c>
     </row>
     <row r="26">
@@ -2150,25 +2150,25 @@
         <v>198</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.455551515151515</v>
+        <v>0.544448484848485</v>
       </c>
       <c r="E29" t="n">
         <v>0.566973320863775</v>
       </c>
       <c r="F29" t="n">
-        <v>-0.2411</v>
+        <v>0.7589</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.348294375</v>
+        <v>0.651705625</v>
       </c>
       <c r="H29" t="n">
         <v>0.30252453</v>
       </c>
       <c r="I29" t="n">
-        <v>-3.3837</v>
+        <v>-2.3837</v>
       </c>
       <c r="J29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" t="n">
         <v>3.3837</v>
@@ -2183,16 +2183,16 @@
         <v>0.0402930393875587</v>
       </c>
       <c r="O29" t="n">
-        <v>-0.5542</v>
+        <v>0.4458</v>
       </c>
       <c r="P29" t="n">
-        <v>-0.2411</v>
+        <v>0.7589</v>
       </c>
       <c r="Q29" t="n">
-        <v>-0.069875</v>
+        <v>0.930125</v>
       </c>
       <c r="R29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -2206,49 +2206,49 @@
         <v>198</v>
       </c>
       <c r="D30" t="n">
-        <v>74.995303030303</v>
+        <v>-25.004696969697</v>
       </c>
       <c r="E30" t="n">
         <v>0.689657944415446</v>
       </c>
       <c r="F30" t="n">
-        <v>75.07</v>
+        <v>-24.93</v>
       </c>
       <c r="G30" t="n">
-        <v>75.0475625</v>
+        <v>-24.9524375</v>
       </c>
       <c r="H30" t="n">
-        <v>0.541148999999992</v>
+        <v>0.541149</v>
       </c>
       <c r="I30" t="n">
-        <v>72.8</v>
+        <v>-27.2</v>
       </c>
       <c r="J30" t="n">
-        <v>76.6</v>
+        <v>-23.4</v>
       </c>
       <c r="K30" t="n">
         <v>3.8</v>
       </c>
       <c r="L30" t="n">
-        <v>-0.884112948353198</v>
+        <v>-0.884112948353181</v>
       </c>
       <c r="M30" t="n">
-        <v>1.61535932391408</v>
+        <v>1.61535932391407</v>
       </c>
       <c r="N30" t="n">
-        <v>0.0490118559299036</v>
+        <v>0.0490118559299037</v>
       </c>
       <c r="O30" t="n">
-        <v>74.7025</v>
+        <v>-25.2975</v>
       </c>
       <c r="P30" t="n">
-        <v>75.07</v>
+        <v>-24.93</v>
       </c>
       <c r="Q30" t="n">
-        <v>75.415</v>
+        <v>-24.585</v>
       </c>
       <c r="R30" t="n">
-        <v>76.6</v>
+        <v>-23.4</v>
       </c>
     </row>
     <row r="31">
@@ -2598,25 +2598,25 @@
         <v>198</v>
       </c>
       <c r="D37" t="n">
-        <v>41.9121212121212</v>
+        <v>-58.0878787878788</v>
       </c>
       <c r="E37" t="n">
         <v>9.91654795765142</v>
       </c>
       <c r="F37" t="n">
-        <v>41.7</v>
+        <v>-58.3</v>
       </c>
       <c r="G37" t="n">
-        <v>41.84125</v>
+        <v>-58.15875</v>
       </c>
       <c r="H37" t="n">
         <v>11.26776</v>
       </c>
       <c r="I37" t="n">
-        <v>19.3</v>
+        <v>-80.7</v>
       </c>
       <c r="J37" t="n">
-        <v>68.5</v>
+        <v>-31.5</v>
       </c>
       <c r="K37" t="n">
         <v>49.2</v>
@@ -2625,22 +2625,22 @@
         <v>0.125555764638885</v>
       </c>
       <c r="M37" t="n">
-        <v>-0.24578332557544</v>
+        <v>-0.245783325575439</v>
       </c>
       <c r="N37" t="n">
         <v>0.70473837611535</v>
       </c>
       <c r="O37" t="n">
-        <v>34.1</v>
+        <v>-65.9</v>
       </c>
       <c r="P37" t="n">
-        <v>41.7</v>
+        <v>-58.3</v>
       </c>
       <c r="Q37" t="n">
-        <v>48.7</v>
+        <v>-51.3</v>
       </c>
       <c r="R37" t="n">
-        <v>68.5</v>
+        <v>-31.5</v>
       </c>
     </row>
     <row r="38">
@@ -2654,49 +2654,49 @@
         <v>198</v>
       </c>
       <c r="D38" t="n">
-        <v>86.9126626262626</v>
+        <v>-13.0873388888889</v>
       </c>
       <c r="E38" t="n">
-        <v>5.75866315063262</v>
+        <v>5.7586626340977</v>
       </c>
       <c r="F38" t="n">
-        <v>87.5971</v>
+        <v>-12.4029</v>
       </c>
       <c r="G38" t="n">
-        <v>87.198710625</v>
+        <v>-12.80129125</v>
       </c>
       <c r="H38" t="n">
         <v>5.58161835</v>
       </c>
       <c r="I38" t="n">
-        <v>69.4404</v>
+        <v>-30.5596</v>
       </c>
       <c r="J38" t="n">
-        <v>97.8688</v>
+        <v>-2.1312</v>
       </c>
       <c r="K38" t="n">
         <v>28.4284</v>
       </c>
       <c r="L38" t="n">
-        <v>-0.484394149660486</v>
+        <v>-0.484393589138627</v>
       </c>
       <c r="M38" t="n">
-        <v>-0.0773257339747482</v>
+        <v>-0.0773252414139582</v>
       </c>
       <c r="N38" t="n">
-        <v>0.409250369655177</v>
+        <v>0.409250332946639</v>
       </c>
       <c r="O38" t="n">
-        <v>83.754175</v>
+        <v>-16.245825</v>
       </c>
       <c r="P38" t="n">
-        <v>87.5971</v>
+        <v>-12.4029</v>
       </c>
       <c r="Q38" t="n">
-        <v>91.193425</v>
+        <v>-8.806575</v>
       </c>
       <c r="R38" t="n">
-        <v>97.8688</v>
+        <v>-2.1312</v>
       </c>
     </row>
     <row r="39">
@@ -2934,25 +2934,25 @@
         <v>198</v>
       </c>
       <c r="D43" t="n">
-        <v>-74.9798858585859</v>
+        <v>25.0201141414141</v>
       </c>
       <c r="E43" t="n">
         <v>6.20925141293518</v>
       </c>
       <c r="F43" t="n">
-        <v>-75.1646</v>
+        <v>24.8354</v>
       </c>
       <c r="G43" t="n">
-        <v>-75.08205875</v>
+        <v>24.91794125</v>
       </c>
       <c r="H43" t="n">
         <v>5.9222457</v>
       </c>
       <c r="I43" t="n">
-        <v>-89.3316</v>
+        <v>10.6684</v>
       </c>
       <c r="J43" t="n">
-        <v>-59.5297</v>
+        <v>40.4703</v>
       </c>
       <c r="K43" t="n">
         <v>29.8019</v>
@@ -2967,16 +2967,16 @@
         <v>0.441272283089956</v>
       </c>
       <c r="O43" t="n">
-        <v>-79.0956</v>
+        <v>20.9044</v>
       </c>
       <c r="P43" t="n">
-        <v>-75.1646</v>
+        <v>24.8354</v>
       </c>
       <c r="Q43" t="n">
-        <v>-70.728675</v>
+        <v>29.271325</v>
       </c>
       <c r="R43" t="n">
-        <v>-59.5297</v>
+        <v>40.4703</v>
       </c>
     </row>
     <row r="44">
@@ -3270,49 +3270,49 @@
         <v>198</v>
       </c>
       <c r="D49" t="n">
-        <v>66.1469696969697</v>
+        <v>-33.8530303030303</v>
       </c>
       <c r="E49" t="n">
         <v>4.60342687505742</v>
       </c>
       <c r="F49" t="n">
-        <v>66.8</v>
+        <v>-33.2</v>
       </c>
       <c r="G49" t="n">
-        <v>66.34125</v>
+        <v>-33.65875</v>
       </c>
       <c r="H49" t="n">
-        <v>5.1891</v>
+        <v>5.18910000000001</v>
       </c>
       <c r="I49" t="n">
-        <v>53.1</v>
+        <v>-46.9</v>
       </c>
       <c r="J49" t="n">
-        <v>74.7</v>
+        <v>-25.3</v>
       </c>
       <c r="K49" t="n">
         <v>21.6</v>
       </c>
       <c r="L49" t="n">
-        <v>-0.42869780841254</v>
+        <v>-0.428697808412544</v>
       </c>
       <c r="M49" t="n">
-        <v>-0.499300335447267</v>
+        <v>-0.499300335447264</v>
       </c>
       <c r="N49" t="n">
         <v>0.327151302484304</v>
       </c>
       <c r="O49" t="n">
-        <v>62.6</v>
+        <v>-37.4</v>
       </c>
       <c r="P49" t="n">
-        <v>66.8</v>
+        <v>-33.2</v>
       </c>
       <c r="Q49" t="n">
-        <v>69.7</v>
+        <v>-30.3</v>
       </c>
       <c r="R49" t="n">
-        <v>74.7</v>
+        <v>-25.3</v>
       </c>
     </row>
     <row r="50">
@@ -3382,25 +3382,25 @@
         <v>198</v>
       </c>
       <c r="D51" t="n">
-        <v>48.9498909090909</v>
+        <v>-51.0501090909091</v>
       </c>
       <c r="E51" t="n">
         <v>14.1627810937994</v>
       </c>
       <c r="F51" t="n">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="G51" t="n">
-        <v>49.971894375</v>
+        <v>-50.028105625</v>
       </c>
       <c r="H51" t="n">
         <v>12.35495058</v>
       </c>
       <c r="I51" t="n">
-        <v>9.0909</v>
+        <v>-90.9091</v>
       </c>
       <c r="J51" t="n">
-        <v>75</v>
+        <v>-25</v>
       </c>
       <c r="K51" t="n">
         <v>65.9091</v>
@@ -3409,22 +3409,22 @@
         <v>-0.64866715731297</v>
       </c>
       <c r="M51" t="n">
-        <v>0.267160685303493</v>
+        <v>0.267160685303492</v>
       </c>
       <c r="N51" t="n">
         <v>1.00650502492858</v>
       </c>
       <c r="O51" t="n">
-        <v>41.3949</v>
+        <v>-58.6051</v>
       </c>
       <c r="P51" t="n">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="Q51" t="n">
-        <v>58.3333</v>
+        <v>-41.6667</v>
       </c>
       <c r="R51" t="n">
-        <v>75</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="52">
@@ -3547,22 +3547,22 @@
         <v>53</v>
       </c>
       <c r="C54" t="n">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D54" t="n">
-        <v>80.9796954314721</v>
+        <v>80.9227272727273</v>
       </c>
       <c r="E54" t="n">
-        <v>19.5550477305349</v>
+        <v>19.521817513277</v>
       </c>
       <c r="F54" t="n">
         <v>80.2</v>
       </c>
       <c r="G54" t="n">
-        <v>81.0566037735849</v>
+        <v>80.985625</v>
       </c>
       <c r="H54" t="n">
-        <v>20.60814</v>
+        <v>20.53401</v>
       </c>
       <c r="I54" t="n">
         <v>31.6</v>
@@ -3574,22 +3574,22 @@
         <v>101.4</v>
       </c>
       <c r="L54" t="n">
-        <v>-0.0208603817438649</v>
+        <v>-0.013125088349585</v>
       </c>
       <c r="M54" t="n">
-        <v>-0.358136750465492</v>
+        <v>-0.353177704531993</v>
       </c>
       <c r="N54" t="n">
-        <v>1.39323946317338</v>
+        <v>1.38735515946472</v>
       </c>
       <c r="O54" t="n">
-        <v>66.8</v>
+        <v>66.875</v>
       </c>
       <c r="P54" t="n">
         <v>80.2</v>
       </c>
       <c r="Q54" t="n">
-        <v>94.5</v>
+        <v>94.45</v>
       </c>
       <c r="R54" t="n">
         <v>133</v>
@@ -3718,49 +3718,49 @@
         <v>198</v>
       </c>
       <c r="D57" t="n">
-        <v>-0.146975757575758</v>
+        <v>-14.697551010101</v>
       </c>
       <c r="E57" t="n">
-        <v>0.096974439660112</v>
+        <v>9.69740557584923</v>
       </c>
       <c r="F57" t="n">
-        <v>-0.1361</v>
+        <v>-13.6129</v>
       </c>
       <c r="G57" t="n">
-        <v>-0.143185</v>
+        <v>-14.31862125</v>
       </c>
       <c r="H57" t="n">
-        <v>0.11897865</v>
+        <v>11.90512974</v>
       </c>
       <c r="I57" t="n">
-        <v>-0.4234</v>
+        <v>-42.3358</v>
       </c>
       <c r="J57" t="n">
-        <v>-0.0015</v>
+        <v>-0.1459</v>
       </c>
       <c r="K57" t="n">
-        <v>0.4219</v>
+        <v>42.1899</v>
       </c>
       <c r="L57" t="n">
-        <v>-0.29705352868063</v>
+        <v>-0.297055409708941</v>
       </c>
       <c r="M57" t="n">
-        <v>-0.789948571131085</v>
+        <v>-0.790004512241786</v>
       </c>
       <c r="N57" t="n">
-        <v>0.00689167333457327</v>
+        <v>0.689164605187315</v>
       </c>
       <c r="O57" t="n">
-        <v>-0.219375</v>
+        <v>-21.94075</v>
       </c>
       <c r="P57" t="n">
-        <v>-0.1361</v>
+        <v>-13.6129</v>
       </c>
       <c r="Q57" t="n">
-        <v>-0.071175</v>
+        <v>-7.118975</v>
       </c>
       <c r="R57" t="n">
-        <v>-0.0015</v>
+        <v>-0.1459</v>
       </c>
     </row>
     <row r="58">
@@ -3774,49 +3774,49 @@
         <v>198</v>
       </c>
       <c r="D58" t="n">
-        <v>-1.08128686868687</v>
+        <v>-108.128758080808</v>
       </c>
       <c r="E58" t="n">
-        <v>0.0784383195828263</v>
+        <v>7.84400781568312</v>
       </c>
       <c r="F58" t="n">
-        <v>-1.0841</v>
+        <v>-108.4105</v>
       </c>
       <c r="G58" t="n">
-        <v>-1.0795625</v>
+        <v>-107.9563725</v>
       </c>
       <c r="H58" t="n">
-        <v>0.0855460200000001</v>
+        <v>8.55430547999999</v>
       </c>
       <c r="I58" t="n">
-        <v>-1.2659</v>
+        <v>-126.5916</v>
       </c>
       <c r="J58" t="n">
-        <v>-0.9089</v>
+        <v>-90.8852</v>
       </c>
       <c r="K58" t="n">
-        <v>0.357</v>
+        <v>35.7064</v>
       </c>
       <c r="L58" t="n">
-        <v>-0.139373343691161</v>
+        <v>-0.139306013846975</v>
       </c>
       <c r="M58" t="n">
-        <v>-0.742062439906256</v>
+        <v>-0.742058031615904</v>
       </c>
       <c r="N58" t="n">
-        <v>0.00557436864159629</v>
+        <v>0.557449361800882</v>
       </c>
       <c r="O58" t="n">
-        <v>-1.140425</v>
+        <v>-114.0457</v>
       </c>
       <c r="P58" t="n">
-        <v>-1.0841</v>
+        <v>-108.4105</v>
       </c>
       <c r="Q58" t="n">
-        <v>-1.024</v>
+        <v>-102.396275</v>
       </c>
       <c r="R58" t="n">
-        <v>-0.9089</v>
+        <v>-90.8852</v>
       </c>
     </row>
     <row r="59">
@@ -3827,19 +3827,19 @@
         <v>58</v>
       </c>
       <c r="C59" t="n">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D59" t="n">
-        <v>134.505102040816</v>
+        <v>134.152284263959</v>
       </c>
       <c r="E59" t="n">
-        <v>379.846790942375</v>
+        <v>378.908915818964</v>
       </c>
       <c r="F59" t="n">
         <v>52</v>
       </c>
       <c r="G59" t="n">
-        <v>55.3607594936709</v>
+        <v>55.4213836477987</v>
       </c>
       <c r="H59" t="n">
         <v>47.4432</v>
@@ -3854,16 +3854,16 @@
         <v>2341</v>
       </c>
       <c r="L59" t="n">
-        <v>5.07199820134883</v>
+        <v>5.08656419719666</v>
       </c>
       <c r="M59" t="n">
-        <v>25.1186647069904</v>
+        <v>25.2728902908518</v>
       </c>
       <c r="N59" t="n">
-        <v>27.1319136387411</v>
+        <v>26.9961424662183</v>
       </c>
       <c r="O59" t="n">
-        <v>20.75</v>
+        <v>21</v>
       </c>
       <c r="P59" t="n">
         <v>52</v>

</xml_diff>